<commit_message>
Clean math, first step
</commit_message>
<xml_diff>
--- a/about/ekliptik.xlsx
+++ b/about/ekliptik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonastochtermann/Documents/reactProjects/astro-clock/about/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2FD66EED-003D-C849-8925-6327F009F68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{228F2845-C754-5449-BA43-4A9898E25EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="3000" windowWidth="27040" windowHeight="11740" activeTab="1" xr2:uid="{7E12C8DC-D8B5-FD4B-BED9-56792C3EA6CE}"/>
   </bookViews>
@@ -147,10 +147,28 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <start/>
       <end/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
       <top/>
       <bottom/>
       <diagonal/>
@@ -159,9 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -499,7 +519,7 @@
   <dimension ref="A1:I362"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I272" sqref="I272"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1230,7 +1250,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21">
@@ -13892,8 +13912,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DDE213-E5C0-5B43-BCE6-522EA01EA5AA}">
   <dimension ref="A1:AV368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P256" sqref="P256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26241,7 +26262,7 @@
         <f t="shared" si="110"/>
         <v>5.5190004347831396E-3</v>
       </c>
-      <c r="AQ80">
+      <c r="AQ80" s="2">
         <f t="shared" si="97"/>
         <v>2.392405781215249E-3</v>
       </c>

</xml_diff>